<commit_message>
CSV files for all campaign contributions from 2018 to 2022 to ballot committee.
Corporate_contributions filters by corporation.
</commit_message>
<xml_diff>
--- a/BallotQuestions2022Data/Question1/Coalition_to_Stop_the_Tax_Hike_Amendment.xlsx
+++ b/BallotQuestions2022Data/Question1/Coalition_to_Stop_the_Tax_Hike_Amendment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aaryan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aaryan/Desktop/PID/Campaign_Finance_Data/BallotQuestions2022Data/Question1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E18911D-0F72-674A-A2F5-508F5CA341DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5324C80C-6DD6-4D42-BB15-D8C1E4D94F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5881" uniqueCount="1502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5880" uniqueCount="1501">
   <si>
     <t>Date</t>
   </si>
@@ -4526,9 +4526,6 @@
   </si>
   <si>
     <t>CO-CEO</t>
-  </si>
-  <si>
-    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -4910,7 +4907,7 @@
   <dimension ref="A1:R452"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4977,9 +4974,7 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>1501</v>
-      </c>
+      <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">

</xml_diff>